<commit_message>
feature:added eda plots; more to come
</commit_message>
<xml_diff>
--- a/Data form (Responses).xlsx
+++ b/Data form (Responses).xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdul.wasay\Documents\minal_ahmad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2A0B4D-22D0-44A4-BB78-C76EC7088A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Form Responses 1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -23,151 +28,151 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="76">
   <si>
-    <t xml:space="preserve">Timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Handover Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Method of delivering information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time at the start of Handover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time at the end of Handover</t>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Handover Type</t>
+  </si>
+  <si>
+    <t>Method of delivering information</t>
+  </si>
+  <si>
+    <t>Time at the start of Handover</t>
+  </si>
+  <si>
+    <t>Time at the end of Handover</t>
   </si>
   <si>
     <t xml:space="preserve">No. Of cases discussed </t>
   </si>
   <si>
-    <t xml:space="preserve">Total Number of doctors present on shift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of staff attending</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designation of doctor presenting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designation of Antendees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absent from meeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description of SITUATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description of BACKGROUND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description of ASSESSMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description of RECOMMENDATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interruption during handover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verbal, Bluespeir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHO, REGISTRAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHO, FY2, Registrar, Comsultant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excellent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hand Written Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On Call SHO, On Call Registrar, Outliers SHO, Coombs Ward SHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hand Written Note, Verbal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On Call Registrar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very Good</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hand Written Note, Verbal, Email, Bluespeir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coombs Ward SHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verbal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On Call Registrar, Post Night SHO, Outliers SHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hand Written Note, Verbal, Bluespeir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FY2, REGISTRAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FY2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHO, FY2, Registrar</t>
+    <t>Total Number of doctors present on shift</t>
+  </si>
+  <si>
+    <t>Number of staff attending</t>
+  </si>
+  <si>
+    <t>Designation of doctor presenting</t>
+  </si>
+  <si>
+    <t>Designation of Antendees</t>
+  </si>
+  <si>
+    <t>Absent from meeting</t>
+  </si>
+  <si>
+    <t>Description of SITUATION</t>
+  </si>
+  <si>
+    <t>Description of BACKGROUND</t>
+  </si>
+  <si>
+    <t>Description of ASSESSMENT</t>
+  </si>
+  <si>
+    <t>Description of RECOMMENDATION</t>
+  </si>
+  <si>
+    <t>Interruption during handover</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Verbal, Bluespeir</t>
+  </si>
+  <si>
+    <t>SHO, REGISTRAR</t>
+  </si>
+  <si>
+    <t>SHO, FY2, Registrar, Comsultant</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Evening</t>
+  </si>
+  <si>
+    <t>Hand Written Note</t>
+  </si>
+  <si>
+    <t>SHO</t>
+  </si>
+  <si>
+    <t>On Call SHO, On Call Registrar, Outliers SHO, Coombs Ward SHO</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>Night</t>
+  </si>
+  <si>
+    <t>Hand Written Note, Verbal</t>
+  </si>
+  <si>
+    <t>On Call Registrar</t>
+  </si>
+  <si>
+    <t>Very Good</t>
+  </si>
+  <si>
+    <t>Hand Written Note, Verbal, Email, Bluespeir</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>Coombs Ward SHO</t>
+  </si>
+  <si>
+    <t>Verbal</t>
+  </si>
+  <si>
+    <t>On Call Registrar, Post Night SHO, Outliers SHO</t>
+  </si>
+  <si>
+    <t>Hand Written Note, Verbal, Bluespeir</t>
+  </si>
+  <si>
+    <t>FY2, REGISTRAR</t>
+  </si>
+  <si>
+    <t>FY2</t>
+  </si>
+  <si>
+    <t>SHO, FY2, Registrar</t>
   </si>
   <si>
     <t xml:space="preserve">Late start to handover due to unwell patient </t>
   </si>
   <si>
-    <t xml:space="preserve">No handover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHO, Registrar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Late start due to unknown reasons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verbal,  Email, Bluespeir</t>
+    <t>No handover</t>
+  </si>
+  <si>
+    <t>SHO, Registrar</t>
+  </si>
+  <si>
+    <t>Late start due to unknown reasons</t>
+  </si>
+  <si>
+    <t>Verbal,  Email, Bluespeir</t>
   </si>
   <si>
     <t xml:space="preserve">No handover </t>
@@ -176,127 +181,106 @@
     <t xml:space="preserve">None </t>
   </si>
   <si>
-    <t xml:space="preserve">On Call SHO, On Call Registrar, Post Night SHO, Outliers SHO, Coombs Ward SHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTRAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attempts at making consultant to consultant referrals during meeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verbal, Email, Bluespier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHO, FY2, REGISTRAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHO, FY2, Registrar, Consultant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On Call SHO, On Call Registrar, Post Night SHO, Outliers SHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On Call Registrar, Coombs Ward SHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHO, Registrar, Comsultant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consultation calls over the phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bleeps from A+E, Urgent need to review patient</t>
+    <t>On Call SHO, On Call Registrar, Post Night SHO, Outliers SHO, Coombs Ward SHO</t>
+  </si>
+  <si>
+    <t>REGISTRAR</t>
+  </si>
+  <si>
+    <t>Attempts at making consultant to consultant referrals during meeting</t>
+  </si>
+  <si>
+    <t>Verbal, Email, Bluespier</t>
+  </si>
+  <si>
+    <t>SHO, FY2, REGISTRAR</t>
+  </si>
+  <si>
+    <t>SHO, FY2, Registrar, Consultant</t>
+  </si>
+  <si>
+    <t>On Call SHO, On Call Registrar, Post Night SHO, Outliers SHO</t>
+  </si>
+  <si>
+    <t>On Call Registrar, Coombs Ward SHO</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>SHO, Registrar, Comsultant</t>
+  </si>
+  <si>
+    <t>Consultation calls over the phone</t>
+  </si>
+  <si>
+    <t>Bleeps from A+E, Urgent need to review patient</t>
   </si>
   <si>
     <t xml:space="preserve"> nil</t>
   </si>
   <si>
-    <t xml:space="preserve">Post Night SHO, Coombs Ward SHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personal anecdotes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verbal, Bluespier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hand Written Note, Verbal, Email, Bluespier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">discussion regarding availability of scrub kits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHO, FY2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On Call Registrar, Outliers SHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Late arrival of Night Sho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHO, Registrar, Consultant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Team in theaters delayed handover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delayed start due to trauma call</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hand Written Note, Verbal, Email</t>
+    <t>Post Night SHO, Coombs Ward SHO</t>
+  </si>
+  <si>
+    <t>Personal anecdotes</t>
+  </si>
+  <si>
+    <t>Verbal, Bluespier</t>
+  </si>
+  <si>
+    <t>Hand Written Note, Verbal, Email, Bluespier</t>
+  </si>
+  <si>
+    <t>discussion regarding availability of scrub kits</t>
+  </si>
+  <si>
+    <t>SHO, FY2</t>
+  </si>
+  <si>
+    <t>On Call Registrar, Outliers SHO</t>
+  </si>
+  <si>
+    <t>Late arrival of Night Sho</t>
+  </si>
+  <si>
+    <t>SHO, Registrar, Consultant</t>
+  </si>
+  <si>
+    <t>Team in theaters delayed handover</t>
+  </si>
+  <si>
+    <t>Delayed start due to trauma call</t>
+  </si>
+  <si>
+    <t>Hand Written Note, Verbal, Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="167" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF434343"/>
       <name val="Roboto"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -321,14 +305,14 @@
     </fill>
   </fills>
   <borders count="13">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF442F65"/>
       </left>
@@ -343,7 +327,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF5B3F86"/>
       </left>
@@ -358,7 +342,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF5B3F86"/>
       </left>
@@ -373,7 +357,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF442F65"/>
       </left>
@@ -388,7 +372,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
@@ -403,7 +387,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
@@ -418,7 +402,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF442F65"/>
       </left>
@@ -433,7 +417,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFF8F9FA"/>
       </left>
@@ -448,7 +432,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFF8F9FA"/>
       </left>
@@ -463,7 +447,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF442F65"/>
       </left>
@@ -478,7 +462,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFF8F9FA"/>
       </left>
@@ -493,7 +477,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFF8F9FA"/>
       </left>
@@ -509,226 +493,111 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="41">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="42">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="19" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="19" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="19" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="19" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="19" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="19" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="19" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF7F7F7"/>
-          <bgColor rgb="FF272727"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -787,141 +656,474 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF442F65"/>
       <rgbColor rgb="FF434343"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:Q53" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:Q53" totalsRowShown="0">
   <tableColumns count="17">
-    <tableColumn id="1" name="Timestamp"/>
-    <tableColumn id="2" name="Date"/>
-    <tableColumn id="3" name="Handover Type"/>
-    <tableColumn id="4" name="Method of delivering information"/>
-    <tableColumn id="5" name="Time at the start of Handover"/>
-    <tableColumn id="6" name="Time at the end of Handover"/>
-    <tableColumn id="7" name="No. Of cases discussed "/>
-    <tableColumn id="8" name="Total Number of doctors present on shift"/>
-    <tableColumn id="9" name="Number of staff attending"/>
-    <tableColumn id="10" name="Designation of doctor presenting"/>
-    <tableColumn id="11" name="Designation of Antendees"/>
-    <tableColumn id="12" name="Absent from meeting"/>
-    <tableColumn id="13" name="Description of SITUATION"/>
-    <tableColumn id="14" name="Description of BACKGROUND"/>
-    <tableColumn id="15" name="Description of ASSESSMENT"/>
-    <tableColumn id="16" name="Description of RECOMMENDATION"/>
-    <tableColumn id="17" name="Interruption during handover"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Timestamp"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Date"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Handover Type"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Method of delivering information"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Time at the start of Handover"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Time at the end of Handover"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="No. Of cases discussed "/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Total Number of doctors present on shift"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Number of staff attending"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Designation of doctor presenting"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Designation of Antendees"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Absent from meeting"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Description of SITUATION"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Description of BACKGROUND"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Description of ASSESSMENT"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Description of RECOMMENDATION"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Interruption during handover"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_1" displayName="Table_1" ref="A54:Q54" headerRowCount="0" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_1" displayName="Table_1" ref="A54:Q54" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="17">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-    <tableColumn id="8" name="Column8"/>
-    <tableColumn id="9" name="Column9"/>
-    <tableColumn id="10" name="Column10"/>
-    <tableColumn id="11" name="Column11"/>
-    <tableColumn id="12" name="Column12"/>
-    <tableColumn id="13" name="Column13"/>
-    <tableColumn id="14" name="Column14"/>
-    <tableColumn id="15" name="Column15"/>
-    <tableColumn id="16" name="Column16"/>
-    <tableColumn id="17" name="Column17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Column17"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table_2" displayName="Table_2" ref="A55:Q55" headerRowCount="0" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_2" displayName="Table_2" ref="A55:Q55" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="17">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-    <tableColumn id="8" name="Column8"/>
-    <tableColumn id="9" name="Column9"/>
-    <tableColumn id="10" name="Column10"/>
-    <tableColumn id="11" name="Column11"/>
-    <tableColumn id="12" name="Column12"/>
-    <tableColumn id="13" name="Column13"/>
-    <tableColumn id="14" name="Column14"/>
-    <tableColumn id="15" name="Column15"/>
-    <tableColumn id="16" name="Column16"/>
-    <tableColumn id="17" name="Column17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="Column17"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table_3" displayName="Table_3" ref="B13:R13" headerRowCount="0" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_3" displayName="Table_3" ref="B13:R13" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="17">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-    <tableColumn id="8" name="Column8"/>
-    <tableColumn id="9" name="Column9"/>
-    <tableColumn id="10" name="Column10"/>
-    <tableColumn id="11" name="Column11"/>
-    <tableColumn id="12" name="Column12"/>
-    <tableColumn id="13" name="Column13"/>
-    <tableColumn id="14" name="Column14"/>
-    <tableColumn id="15" name="Column15"/>
-    <tableColumn id="16" name="Column16"/>
-    <tableColumn id="17" name="Column17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="Column17"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="Q20" activeCellId="0" sqref="Q20"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="63.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="58.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="33.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="49.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="53.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="47.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="56.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="50.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="25.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="18" style="0" width="18.88"/>
+    <col min="1" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="55.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" customWidth="1"/>
+    <col min="8" max="8" width="63" customWidth="1"/>
+    <col min="9" max="9" width="58.5703125" customWidth="1"/>
+    <col min="10" max="10" width="41.7109375" customWidth="1"/>
+    <col min="11" max="11" width="37.5703125" customWidth="1"/>
+    <col min="12" max="12" width="49.42578125" customWidth="1"/>
+    <col min="13" max="13" width="53.28515625" customWidth="1"/>
+    <col min="14" max="14" width="47.28515625" customWidth="1"/>
+    <col min="15" max="15" width="56.140625" customWidth="1"/>
+    <col min="16" max="16" width="50.42578125" customWidth="1"/>
+    <col min="17" max="17" width="46.42578125" customWidth="1"/>
+    <col min="18" max="23" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -974,11 +1176,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <v>45518.6936316782</v>
-      </c>
-      <c r="B2" s="5" t="n">
+    <row r="2" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>45518.693631678201</v>
+      </c>
+      <c r="B2" s="5">
         <v>45512</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -987,19 +1189,19 @@
       <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F2" s="7" t="n">
+      <c r="E2" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F2" s="7">
         <v>0.375</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="6">
         <v>34</v>
       </c>
-      <c r="H2" s="6" t="n">
+      <c r="H2" s="6">
         <v>10</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="6">
         <v>10</v>
       </c>
       <c r="J2" s="6" t="s">
@@ -1025,11 +1227,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
-        <v>45551.7786426273</v>
-      </c>
-      <c r="B3" s="10" t="n">
+    <row r="3" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>45551.778642627301</v>
+      </c>
+      <c r="B3" s="10">
         <v>45512</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1038,19 +1240,19 @@
       <c r="D3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="12" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="F3" s="12" t="n">
+      <c r="E3" s="12">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="F3" s="12">
         <v>0.711805555554747</v>
       </c>
-      <c r="G3" s="11" t="n">
+      <c r="G3" s="11">
         <v>4</v>
       </c>
-      <c r="H3" s="11" t="n">
+      <c r="H3" s="11">
         <v>10</v>
       </c>
-      <c r="I3" s="11" t="n">
+      <c r="I3" s="11">
         <v>1</v>
       </c>
       <c r="J3" s="11" t="s">
@@ -1078,11 +1280,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>45585.536269294</v>
-      </c>
-      <c r="B4" s="5" t="n">
+    <row r="4" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>45585.536269294003</v>
+      </c>
+      <c r="B4" s="5">
         <v>45512</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1091,19 +1293,19 @@
       <c r="D4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="7" t="n">
-        <v>0.840277777781012</v>
-      </c>
-      <c r="F4" s="7" t="n">
+      <c r="E4" s="7">
+        <v>0.84027777778101198</v>
+      </c>
+      <c r="F4" s="7">
         <v>0.850694444445253</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="6">
         <v>5</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H4" s="6">
         <v>3</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="6">
         <v>2</v>
       </c>
       <c r="J4" s="6" t="s">
@@ -1131,11 +1333,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="n">
-        <v>45551.7802770949</v>
-      </c>
-      <c r="B5" s="10" t="n">
+    <row r="5" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>45551.780277094898</v>
+      </c>
+      <c r="B5" s="10">
         <v>45513</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1144,13 +1346,13 @@
       <c r="D5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="12" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F5" s="12" t="n">
-        <v>0.416666666664241</v>
-      </c>
-      <c r="G5" s="11" t="n">
+      <c r="E5" s="12">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.41666666666424101</v>
+      </c>
+      <c r="G5" s="11">
         <v>36</v>
       </c>
       <c r="H5" s="11" t="s">
@@ -1184,11 +1386,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
-        <v>45551.7814166204</v>
-      </c>
-      <c r="B6" s="5" t="n">
+    <row r="6" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>45551.781416620397</v>
+      </c>
+      <c r="B6" s="5">
         <v>45513</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1197,19 +1399,19 @@
       <c r="D6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="7">
         <v>0.84375</v>
       </c>
-      <c r="F6" s="7" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="G6" s="6" t="n">
+      <c r="F6" s="7">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="G6" s="6">
         <v>4</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="6">
         <v>3</v>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I6" s="6">
         <v>2</v>
       </c>
       <c r="J6" s="6" t="s">
@@ -1237,11 +1439,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="n">
-        <v>45585.5372411921</v>
-      </c>
-      <c r="B7" s="10" t="n">
+    <row r="7" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>45585.537241192098</v>
+      </c>
+      <c r="B7" s="10">
         <v>45513</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -1250,19 +1452,19 @@
       <c r="D7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="12" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="F7" s="12" t="n">
-        <v>0.718055555553292</v>
-      </c>
-      <c r="G7" s="11" t="n">
+      <c r="E7" s="12">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0.71805555555329204</v>
+      </c>
+      <c r="G7" s="11">
         <v>2</v>
       </c>
-      <c r="H7" s="11" t="n">
+      <c r="H7" s="11">
         <v>10</v>
       </c>
-      <c r="I7" s="11" t="n">
+      <c r="I7" s="11">
         <v>2</v>
       </c>
       <c r="J7" s="11" t="s">
@@ -1290,11 +1492,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
-        <v>45585.5382381134</v>
-      </c>
-      <c r="B8" s="5" t="n">
+    <row r="8" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>45585.538238113397</v>
+      </c>
+      <c r="B8" s="5">
         <v>45514</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1303,19 +1505,19 @@
       <c r="D8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <v>0.361111111109494</v>
-      </c>
-      <c r="G8" s="6" t="n">
+      <c r="E8" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.36111111110949401</v>
+      </c>
+      <c r="G8" s="6">
         <v>7</v>
       </c>
-      <c r="H8" s="6" t="n">
+      <c r="H8" s="6">
         <v>6</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I8" s="6">
         <v>6</v>
       </c>
       <c r="J8" s="6" t="s">
@@ -1341,11 +1543,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="n">
-        <v>45585.5398058333</v>
-      </c>
-      <c r="B9" s="10" t="n">
+    <row r="9" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>45585.539805833301</v>
+      </c>
+      <c r="B9" s="10">
         <v>45514</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -1354,19 +1556,19 @@
       <c r="D9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="12" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="F9" s="12" t="n">
-        <v>0.864583333335759</v>
-      </c>
-      <c r="G9" s="11" t="n">
+      <c r="E9" s="12">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.86458333333575899</v>
+      </c>
+      <c r="G9" s="11">
         <v>4</v>
       </c>
-      <c r="H9" s="11" t="n">
+      <c r="H9" s="11">
         <v>3</v>
       </c>
-      <c r="I9" s="11" t="n">
+      <c r="I9" s="11">
         <v>3</v>
       </c>
       <c r="J9" s="11" t="s">
@@ -1392,11 +1594,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
-        <v>45585.5508097222</v>
-      </c>
-      <c r="B10" s="5" t="n">
+    <row r="10" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>45585.550809722197</v>
+      </c>
+      <c r="B10" s="5">
         <v>45515</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1405,19 +1607,19 @@
       <c r="D10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F10" s="7" t="n">
+      <c r="E10" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F10" s="7">
         <v>0.350694444445253</v>
       </c>
-      <c r="G10" s="6" t="n">
+      <c r="G10" s="6">
         <v>7</v>
       </c>
-      <c r="H10" s="6" t="n">
+      <c r="H10" s="6">
         <v>6</v>
       </c>
-      <c r="I10" s="6" t="n">
+      <c r="I10" s="6">
         <v>6</v>
       </c>
       <c r="J10" s="6" t="s">
@@ -1441,11 +1643,11 @@
       </c>
       <c r="Q10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="n">
-        <v>45585.5517788889</v>
-      </c>
-      <c r="B11" s="10" t="n">
+    <row r="11" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>45585.551778888897</v>
+      </c>
+      <c r="B11" s="10">
         <v>45515</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1454,19 +1656,19 @@
       <c r="D11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="12" t="n">
+      <c r="E11" s="12">
         <v>0.84375</v>
       </c>
-      <c r="F11" s="12" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="G11" s="11" t="n">
+      <c r="F11" s="12">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="G11" s="11">
         <v>3</v>
       </c>
-      <c r="H11" s="11" t="n">
+      <c r="H11" s="11">
         <v>3</v>
       </c>
-      <c r="I11" s="11" t="n">
+      <c r="I11" s="11">
         <v>2</v>
       </c>
       <c r="J11" s="11" t="s">
@@ -1492,11 +1694,11 @@
       </c>
       <c r="Q11" s="13"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="n">
+    <row r="12" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <v>45585.5539274537</v>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="5">
         <v>45516</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1505,19 +1707,19 @@
       <c r="D12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F12" s="7" t="n">
-        <v>0.427083333335759</v>
-      </c>
-      <c r="G12" s="6" t="n">
+      <c r="E12" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.42708333333575899</v>
+      </c>
+      <c r="G12" s="6">
         <v>35</v>
       </c>
-      <c r="H12" s="6" t="n">
+      <c r="H12" s="6">
         <v>9</v>
       </c>
-      <c r="I12" s="6" t="n">
+      <c r="I12" s="6">
         <v>7</v>
       </c>
       <c r="J12" s="6" t="s">
@@ -1543,11 +1745,11 @@
       </c>
       <c r="Q12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="n">
-        <v>45585.5553327199</v>
-      </c>
-      <c r="B13" s="10" t="n">
+    <row r="13" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>45585.555332719901</v>
+      </c>
+      <c r="B13" s="10">
         <v>45516</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -1572,11 +1774,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="n">
-        <v>45585.5619040509</v>
-      </c>
-      <c r="B14" s="5" t="n">
+    <row r="14" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>45585.561904050897</v>
+      </c>
+      <c r="B14" s="5">
         <v>45516</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1585,19 +1787,19 @@
       <c r="D14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="7" t="n">
-        <v>0.840277777781012</v>
-      </c>
-      <c r="F14" s="7" t="n">
+      <c r="E14" s="7">
+        <v>0.84027777778101198</v>
+      </c>
+      <c r="F14" s="7">
         <v>0.84375</v>
       </c>
-      <c r="G14" s="6" t="n">
+      <c r="G14" s="6">
         <v>2</v>
       </c>
-      <c r="H14" s="6" t="n">
+      <c r="H14" s="6">
         <v>3</v>
       </c>
-      <c r="I14" s="6" t="n">
+      <c r="I14" s="6">
         <v>3</v>
       </c>
       <c r="J14" s="6" t="s">
@@ -1623,11 +1825,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="n">
-        <v>45518.6936316782</v>
-      </c>
-      <c r="B15" s="10" t="n">
+    <row r="15" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>45518.693631678201</v>
+      </c>
+      <c r="B15" s="10">
         <v>45517</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -1636,19 +1838,19 @@
       <c r="D15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="12" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F15" s="12" t="n">
+      <c r="E15" s="12">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F15" s="12">
         <v>0.375</v>
       </c>
-      <c r="G15" s="11" t="n">
+      <c r="G15" s="11">
         <v>34</v>
       </c>
-      <c r="H15" s="11" t="n">
+      <c r="H15" s="11">
         <v>10</v>
       </c>
-      <c r="I15" s="11" t="n">
+      <c r="I15" s="11">
         <v>10</v>
       </c>
       <c r="J15" s="11" t="s">
@@ -1674,11 +1876,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="n">
-        <v>45551.7786426273</v>
-      </c>
-      <c r="B16" s="5" t="n">
+    <row r="16" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>45551.778642627301</v>
+      </c>
+      <c r="B16" s="5">
         <v>45517</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1687,19 +1889,19 @@
       <c r="D16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="7" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="F16" s="7" t="n">
+      <c r="E16" s="7">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="F16" s="7">
         <v>0.711805555554747</v>
       </c>
-      <c r="G16" s="6" t="n">
+      <c r="G16" s="6">
         <v>4</v>
       </c>
-      <c r="H16" s="6" t="n">
+      <c r="H16" s="6">
         <v>10</v>
       </c>
-      <c r="I16" s="6" t="n">
+      <c r="I16" s="6">
         <v>1</v>
       </c>
       <c r="J16" s="6" t="s">
@@ -1727,11 +1929,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="n">
-        <v>45585.536269294</v>
-      </c>
-      <c r="B17" s="10" t="n">
+    <row r="17" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>45585.536269294003</v>
+      </c>
+      <c r="B17" s="10">
         <v>45517</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -1740,19 +1942,19 @@
       <c r="D17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="12" t="n">
-        <v>0.836805555555556</v>
-      </c>
-      <c r="F17" s="12" t="n">
+      <c r="E17" s="12">
+        <v>0.83680555555555602</v>
+      </c>
+      <c r="F17" s="12">
         <v>0.850694444445253</v>
       </c>
-      <c r="G17" s="11" t="n">
+      <c r="G17" s="11">
         <v>3</v>
       </c>
-      <c r="H17" s="11" t="n">
+      <c r="H17" s="11">
         <v>3</v>
       </c>
-      <c r="I17" s="11" t="n">
+      <c r="I17" s="11">
         <v>2</v>
       </c>
       <c r="J17" s="11" t="s">
@@ -1780,11 +1982,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="n">
-        <v>45518.7148073495</v>
-      </c>
-      <c r="B18" s="5" t="n">
+    <row r="18" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>45518.714807349497</v>
+      </c>
+      <c r="B18" s="5">
         <v>45518</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -1795,13 +1997,13 @@
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="6" t="n">
+      <c r="G18" s="6">
         <v>0</v>
       </c>
-      <c r="H18" s="6" t="n">
+      <c r="H18" s="6">
         <v>10</v>
       </c>
-      <c r="I18" s="6" t="n">
+      <c r="I18" s="6">
         <v>0</v>
       </c>
       <c r="J18" s="6" t="s">
@@ -1827,11 +2029,11 @@
       </c>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="n">
+    <row r="19" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
         <v>45519</v>
       </c>
-      <c r="B19" s="10" t="n">
+      <c r="B19" s="10">
         <v>45518</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -1840,19 +2042,19 @@
       <c r="D19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="12" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F19" s="12" t="n">
+      <c r="E19" s="12">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F19" s="12">
         <v>0.375</v>
       </c>
-      <c r="G19" s="11" t="n">
+      <c r="G19" s="11">
         <v>18</v>
       </c>
-      <c r="H19" s="11" t="n">
+      <c r="H19" s="11">
         <v>10</v>
       </c>
-      <c r="I19" s="11" t="n">
+      <c r="I19" s="11">
         <v>7</v>
       </c>
       <c r="J19" s="11" t="s">
@@ -1880,11 +2082,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="n">
-        <v>45597.1551023843</v>
-      </c>
-      <c r="B20" s="5" t="n">
+    <row r="20" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>45597.155102384299</v>
+      </c>
+      <c r="B20" s="5">
         <v>45519</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1893,19 +2095,19 @@
       <c r="D20" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F20" s="7" t="n">
-        <v>0.427083333335759</v>
-      </c>
-      <c r="G20" s="6" t="n">
+      <c r="E20" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.42708333333575899</v>
+      </c>
+      <c r="G20" s="6">
         <v>60</v>
       </c>
-      <c r="H20" s="6" t="n">
+      <c r="H20" s="6">
         <v>9</v>
       </c>
-      <c r="I20" s="6" t="n">
+      <c r="I20" s="6">
         <v>7</v>
       </c>
       <c r="J20" s="6" t="s">
@@ -1933,11 +2135,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="n">
-        <v>45597.1572603935</v>
-      </c>
-      <c r="B21" s="10" t="n">
+    <row r="21" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>45597.157260393498</v>
+      </c>
+      <c r="B21" s="10">
         <v>45519</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -1946,19 +2148,19 @@
       <c r="D21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="12" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="F21" s="12" t="n">
-        <v>0.715277777781012</v>
-      </c>
-      <c r="G21" s="11" t="n">
+      <c r="E21" s="12">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0.71527777778101198</v>
+      </c>
+      <c r="G21" s="11">
         <v>5</v>
       </c>
-      <c r="H21" s="11" t="n">
+      <c r="H21" s="11">
         <v>9</v>
       </c>
-      <c r="I21" s="11" t="n">
+      <c r="I21" s="11">
         <v>2</v>
       </c>
       <c r="J21" s="11" t="s">
@@ -1986,11 +2188,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="n">
-        <v>45520.4142816088</v>
-      </c>
-      <c r="B22" s="5" t="n">
+    <row r="22" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>45520.414281608799</v>
+      </c>
+      <c r="B22" s="5">
         <v>45520</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1999,19 +2201,19 @@
       <c r="D22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F22" s="7" t="n">
+      <c r="E22" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F22" s="7">
         <v>0.413194444445253</v>
       </c>
-      <c r="G22" s="6" t="n">
-        <v>33</v>
-      </c>
-      <c r="H22" s="6" t="n">
+      <c r="G22" s="6">
+        <v>33</v>
+      </c>
+      <c r="H22" s="6">
         <v>10</v>
       </c>
-      <c r="I22" s="6" t="n">
+      <c r="I22" s="6">
         <v>8</v>
       </c>
       <c r="J22" s="6" t="s">
@@ -2039,11 +2241,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="n">
-        <v>45597.1583084028</v>
-      </c>
-      <c r="B23" s="10" t="n">
+    <row r="23" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>45597.158308402803</v>
+      </c>
+      <c r="B23" s="10">
         <v>45520</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -2052,19 +2254,19 @@
       <c r="D23" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="12" t="n">
-        <v>0.840277777781012</v>
-      </c>
-      <c r="F23" s="12" t="n">
+      <c r="E23" s="12">
+        <v>0.84027777778101198</v>
+      </c>
+      <c r="F23" s="12">
         <v>0.850694444445253</v>
       </c>
-      <c r="G23" s="11" t="n">
+      <c r="G23" s="11">
         <v>9</v>
       </c>
-      <c r="H23" s="11" t="n">
+      <c r="H23" s="11">
         <v>3</v>
       </c>
-      <c r="I23" s="11" t="n">
+      <c r="I23" s="11">
         <v>3</v>
       </c>
       <c r="J23" s="11" t="s">
@@ -2089,11 +2291,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="n">
-        <v>45597.1653558681</v>
-      </c>
-      <c r="B24" s="5" t="n">
+    <row r="24" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>45597.165355868099</v>
+      </c>
+      <c r="B24" s="5">
         <v>45521</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -2102,16 +2304,16 @@
       <c r="D24" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F24" s="7" t="n">
-        <v>0.416666666664241</v>
-      </c>
-      <c r="H24" s="6" t="n">
+      <c r="E24" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.41666666666424101</v>
+      </c>
+      <c r="H24" s="6">
         <v>8</v>
       </c>
-      <c r="I24" s="6" t="n">
+      <c r="I24" s="6">
         <v>6</v>
       </c>
       <c r="J24" s="6" t="s">
@@ -2139,11 +2341,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="n">
-        <v>45597.1663031713</v>
-      </c>
-      <c r="B25" s="10" t="n">
+    <row r="25" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="9">
+        <v>45597.166303171303</v>
+      </c>
+      <c r="B25" s="10">
         <v>45521</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -2152,19 +2354,19 @@
       <c r="D25" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="12" t="n">
-        <v>0.841666666667152</v>
-      </c>
-      <c r="F25" s="12" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="G25" s="11" t="n">
+      <c r="E25" s="12">
+        <v>0.84166666666715195</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="G25" s="11">
         <v>4</v>
       </c>
-      <c r="H25" s="11" t="n">
+      <c r="H25" s="11">
         <v>3</v>
       </c>
-      <c r="I25" s="11" t="n">
+      <c r="I25" s="11">
         <v>2</v>
       </c>
       <c r="J25" s="11" t="s">
@@ -2192,11 +2394,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="n">
-        <v>45597.170482338</v>
-      </c>
-      <c r="B26" s="5" t="n">
+    <row r="26" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>45597.170482337999</v>
+      </c>
+      <c r="B26" s="5">
         <v>45522</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -2205,19 +2407,19 @@
       <c r="D26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F26" s="7" t="n">
-        <v>0.364583333335759</v>
-      </c>
-      <c r="G26" s="6" t="n">
+      <c r="E26" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.36458333333575899</v>
+      </c>
+      <c r="G26" s="6">
         <v>12</v>
       </c>
-      <c r="H26" s="6" t="n">
+      <c r="H26" s="6">
         <v>5</v>
       </c>
-      <c r="I26" s="6" t="n">
+      <c r="I26" s="6">
         <v>5</v>
       </c>
       <c r="J26" s="6" t="s">
@@ -2245,11 +2447,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="n">
-        <v>45597.1712240741</v>
-      </c>
-      <c r="B27" s="10" t="n">
+    <row r="27" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>45597.171224074104</v>
+      </c>
+      <c r="B27" s="10">
         <v>45522</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2258,19 +2460,19 @@
       <c r="D27" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="12" t="n">
+      <c r="E27" s="12">
         <v>0.84375</v>
       </c>
-      <c r="F27" s="12" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="G27" s="11" t="n">
+      <c r="F27" s="12">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="G27" s="11">
         <v>6</v>
       </c>
-      <c r="H27" s="11" t="n">
+      <c r="H27" s="11">
         <v>3</v>
       </c>
-      <c r="I27" s="11" t="n">
+      <c r="I27" s="11">
         <v>3</v>
       </c>
       <c r="J27" s="11" t="s">
@@ -2295,11 +2497,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="n">
+    <row r="28" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
         <v>45525.3452222454</v>
       </c>
-      <c r="B28" s="5" t="n">
+      <c r="B28" s="5">
         <v>45523</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -2308,19 +2510,19 @@
       <c r="D28" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="7" t="n">
-        <v>0.340277777781012</v>
-      </c>
-      <c r="F28" s="7" t="n">
-        <v>0.385416666664241</v>
-      </c>
-      <c r="G28" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="H28" s="6" t="n">
+      <c r="E28" s="7">
+        <v>0.34027777778101198</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0.38541666666424101</v>
+      </c>
+      <c r="G28" s="6">
+        <v>22</v>
+      </c>
+      <c r="H28" s="6">
         <v>10</v>
       </c>
-      <c r="I28" s="6" t="n">
+      <c r="I28" s="6">
         <v>9</v>
       </c>
       <c r="J28" s="6" t="s">
@@ -2348,11 +2550,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="n">
-        <v>45604.0509585995</v>
-      </c>
-      <c r="B29" s="10" t="n">
+    <row r="29" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>45604.050958599502</v>
+      </c>
+      <c r="B29" s="10">
         <v>45524</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -2361,19 +2563,19 @@
       <c r="D29" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="12" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F29" s="12" t="n">
+      <c r="E29" s="12">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F29" s="12">
         <v>0.444444444445253</v>
       </c>
-      <c r="G29" s="11" t="n">
+      <c r="G29" s="11">
         <v>40</v>
       </c>
-      <c r="H29" s="11" t="n">
+      <c r="H29" s="11">
         <v>7</v>
       </c>
-      <c r="I29" s="11" t="n">
+      <c r="I29" s="11">
         <v>6</v>
       </c>
       <c r="J29" s="11" t="s">
@@ -2398,11 +2600,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="n">
-        <v>45604.0492114815</v>
-      </c>
-      <c r="B30" s="5" t="n">
+    <row r="30" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>45604.049211481499</v>
+      </c>
+      <c r="B30" s="5">
         <v>45524</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -2411,19 +2613,19 @@
       <c r="D30" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="7" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="F30" s="7" t="n">
-        <v>0.718055555553292</v>
-      </c>
-      <c r="G30" s="6" t="n">
+      <c r="E30" s="7">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0.71805555555329204</v>
+      </c>
+      <c r="G30" s="6">
         <v>2</v>
       </c>
-      <c r="H30" s="6" t="n">
+      <c r="H30" s="6">
         <v>9</v>
       </c>
-      <c r="I30" s="6" t="n">
+      <c r="I30" s="6">
         <v>2</v>
       </c>
       <c r="J30" s="6" t="s">
@@ -2448,11 +2650,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="n">
-        <v>45604.0522225463</v>
-      </c>
-      <c r="B31" s="10" t="n">
+    <row r="31" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>45604.052222546299</v>
+      </c>
+      <c r="B31" s="10">
         <v>45524</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -2461,19 +2663,19 @@
       <c r="D31" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="12" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="F31" s="12" t="n">
-        <v>0.864583333335759</v>
-      </c>
-      <c r="G31" s="11" t="n">
+      <c r="E31" s="12">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="F31" s="12">
+        <v>0.86458333333575899</v>
+      </c>
+      <c r="G31" s="11">
         <v>4</v>
       </c>
-      <c r="H31" s="11" t="n">
+      <c r="H31" s="11">
         <v>3</v>
       </c>
-      <c r="I31" s="11" t="n">
+      <c r="I31" s="11">
         <v>3</v>
       </c>
       <c r="J31" s="11" t="s">
@@ -2495,11 +2697,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="n">
-        <v>45525.4014731597</v>
-      </c>
-      <c r="B32" s="5" t="n">
+    <row r="32" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>45525.401473159698</v>
+      </c>
+      <c r="B32" s="5">
         <v>45525</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -2508,19 +2710,19 @@
       <c r="D32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="7" t="n">
-        <v>0.340277777781012</v>
-      </c>
-      <c r="F32" s="7" t="n">
-        <v>0.402777777781012</v>
-      </c>
-      <c r="G32" s="6" t="n">
+      <c r="E32" s="7">
+        <v>0.34027777778101198</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0.40277777778101198</v>
+      </c>
+      <c r="G32" s="6">
         <v>19</v>
       </c>
-      <c r="H32" s="6" t="n">
+      <c r="H32" s="6">
         <v>12</v>
       </c>
-      <c r="I32" s="6" t="n">
+      <c r="I32" s="6">
         <v>10</v>
       </c>
       <c r="J32" s="6" t="s">
@@ -2548,11 +2750,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="n">
-        <v>45604.0536660764</v>
-      </c>
-      <c r="B33" s="10" t="n">
+    <row r="33" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>45604.053666076397</v>
+      </c>
+      <c r="B33" s="10">
         <v>45526</v>
       </c>
       <c r="C33" s="11" t="s">
@@ -2561,19 +2763,19 @@
       <c r="D33" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="12" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F33" s="12" t="n">
+      <c r="E33" s="12">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F33" s="12">
         <v>0.413194444445253</v>
       </c>
-      <c r="G33" s="11" t="n">
+      <c r="G33" s="11">
         <v>30</v>
       </c>
-      <c r="H33" s="11" t="n">
+      <c r="H33" s="11">
         <v>8</v>
       </c>
-      <c r="I33" s="11" t="n">
+      <c r="I33" s="11">
         <v>10</v>
       </c>
       <c r="J33" s="11" t="s">
@@ -2598,11 +2800,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="n">
-        <v>45604.4934967477</v>
-      </c>
-      <c r="B34" s="5" t="n">
+    <row r="34" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>45604.493496747702</v>
+      </c>
+      <c r="B34" s="5">
         <v>45526</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -2611,19 +2813,19 @@
       <c r="D34" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="7" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="F34" s="7" t="n">
-        <v>0.715277777781012</v>
-      </c>
-      <c r="G34" s="6" t="n">
+      <c r="E34" s="7">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0.71527777778101198</v>
+      </c>
+      <c r="G34" s="6">
         <v>6</v>
       </c>
-      <c r="H34" s="6" t="n">
+      <c r="H34" s="6">
         <v>9</v>
       </c>
-      <c r="I34" s="6" t="n">
+      <c r="I34" s="6">
         <v>4</v>
       </c>
       <c r="J34" s="6" t="s">
@@ -2648,11 +2850,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="n">
+    <row r="35" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
         <v>45604.4956289931</v>
       </c>
-      <c r="B35" s="10" t="n">
+      <c r="B35" s="10">
         <v>45526</v>
       </c>
       <c r="C35" s="11" t="s">
@@ -2661,19 +2863,19 @@
       <c r="D35" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="12" t="n">
-        <v>0.840277777781012</v>
-      </c>
-      <c r="F35" s="12" t="n">
+      <c r="E35" s="12">
+        <v>0.84027777778101198</v>
+      </c>
+      <c r="F35" s="12">
         <v>0.850694444445253</v>
       </c>
-      <c r="G35" s="11" t="n">
+      <c r="G35" s="11">
         <v>4</v>
       </c>
-      <c r="H35" s="11" t="n">
+      <c r="H35" s="11">
         <v>3</v>
       </c>
-      <c r="I35" s="11" t="n">
+      <c r="I35" s="11">
         <v>3</v>
       </c>
       <c r="J35" s="11" t="s">
@@ -2695,11 +2897,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="n">
-        <v>45604.4969268171</v>
-      </c>
-      <c r="B36" s="5" t="n">
+    <row r="36" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>45604.496926817097</v>
+      </c>
+      <c r="B36" s="5">
         <v>45527</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -2708,19 +2910,19 @@
       <c r="D36" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F36" s="7" t="n">
-        <v>0.416666666664241</v>
-      </c>
-      <c r="G36" s="6" t="n">
+      <c r="E36" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0.41666666666424101</v>
+      </c>
+      <c r="G36" s="6">
         <v>35</v>
       </c>
-      <c r="H36" s="6" t="n">
+      <c r="H36" s="6">
         <v>10</v>
       </c>
-      <c r="I36" s="6" t="n">
+      <c r="I36" s="6">
         <v>8</v>
       </c>
       <c r="J36" s="6" t="s">
@@ -2748,11 +2950,11 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="n">
-        <v>45604.4991401042</v>
-      </c>
-      <c r="B37" s="10" t="n">
+    <row r="37" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
+        <v>45604.499140104199</v>
+      </c>
+      <c r="B37" s="10">
         <v>45527</v>
       </c>
       <c r="C37" s="11" t="s">
@@ -2761,19 +2963,19 @@
       <c r="D37" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="12" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="F37" s="12" t="n">
-        <v>0.720138888893416</v>
-      </c>
-      <c r="G37" s="11" t="n">
+      <c r="E37" s="12">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0.72013888889341604</v>
+      </c>
+      <c r="G37" s="11">
         <v>2</v>
       </c>
-      <c r="H37" s="11" t="n">
+      <c r="H37" s="11">
         <v>10</v>
       </c>
-      <c r="I37" s="11" t="n">
+      <c r="I37" s="11">
         <v>3</v>
       </c>
       <c r="J37" s="11" t="s">
@@ -2798,11 +3000,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="n">
-        <v>45604.5075160301</v>
-      </c>
-      <c r="B38" s="5" t="n">
+    <row r="38" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>45604.507516030098</v>
+      </c>
+      <c r="B38" s="5">
         <v>45527</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -2811,19 +3013,19 @@
       <c r="D38" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="7" t="n">
+      <c r="E38" s="7">
         <v>0.84375</v>
       </c>
-      <c r="F38" s="7" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="G38" s="6" t="n">
+      <c r="F38" s="7">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="G38" s="6">
         <v>3</v>
       </c>
-      <c r="H38" s="6" t="n">
+      <c r="H38" s="6">
         <v>3</v>
       </c>
-      <c r="I38" s="6" t="n">
+      <c r="I38" s="6">
         <v>3</v>
       </c>
       <c r="J38" s="6" t="s">
@@ -2848,11 +3050,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="n">
-        <v>45604.5086307407</v>
-      </c>
-      <c r="B39" s="10" t="n">
+    <row r="39" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="9">
+        <v>45604.508630740696</v>
+      </c>
+      <c r="B39" s="10">
         <v>45528</v>
       </c>
       <c r="C39" s="11" t="s">
@@ -2861,19 +3063,19 @@
       <c r="D39" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E39" s="12" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F39" s="12" t="n">
-        <v>0.361111111109494</v>
-      </c>
-      <c r="G39" s="11" t="n">
+      <c r="E39" s="12">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0.36111111110949401</v>
+      </c>
+      <c r="G39" s="11">
         <v>10</v>
       </c>
-      <c r="H39" s="11" t="n">
+      <c r="H39" s="11">
         <v>5</v>
       </c>
-      <c r="I39" s="11" t="n">
+      <c r="I39" s="11">
         <v>5</v>
       </c>
       <c r="J39" s="11" t="s">
@@ -2895,11 +3097,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="n">
-        <v>45604.5092943287</v>
-      </c>
-      <c r="B40" s="5" t="n">
+    <row r="40" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>45604.509294328702</v>
+      </c>
+      <c r="B40" s="5">
         <v>45528</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -2908,19 +3110,19 @@
       <c r="D40" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="7" t="n">
-        <v>0.833333333335759</v>
-      </c>
-      <c r="F40" s="7" t="n">
-        <v>0.843055555553292</v>
-      </c>
-      <c r="G40" s="6" t="n">
+      <c r="E40" s="7">
+        <v>0.83333333333575899</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0.84305555555329204</v>
+      </c>
+      <c r="G40" s="6">
         <v>2</v>
       </c>
-      <c r="H40" s="6" t="n">
+      <c r="H40" s="6">
         <v>3</v>
       </c>
-      <c r="I40" s="6" t="n">
+      <c r="I40" s="6">
         <v>3</v>
       </c>
       <c r="J40" s="6" t="s">
@@ -2942,11 +3144,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="n">
-        <v>45604.5112506366</v>
-      </c>
-      <c r="B41" s="10" t="n">
+    <row r="41" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A41" s="9">
+        <v>45604.511250636599</v>
+      </c>
+      <c r="B41" s="10">
         <v>45529</v>
       </c>
       <c r="C41" s="11" t="s">
@@ -2955,19 +3157,19 @@
       <c r="D41" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="12" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F41" s="12" t="n">
+      <c r="E41" s="12">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F41" s="12">
         <v>0.350694444445253</v>
       </c>
-      <c r="G41" s="11" t="n">
+      <c r="G41" s="11">
         <v>12</v>
       </c>
-      <c r="H41" s="11" t="n">
+      <c r="H41" s="11">
         <v>5</v>
       </c>
-      <c r="I41" s="11" t="n">
+      <c r="I41" s="11">
         <v>4</v>
       </c>
       <c r="J41" s="11" t="s">
@@ -2992,11 +3194,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="n">
-        <v>45604.5215908681</v>
-      </c>
-      <c r="B42" s="5" t="n">
+    <row r="42" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>45604.521590868098</v>
+      </c>
+      <c r="B42" s="5">
         <v>45529</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -3005,19 +3207,19 @@
       <c r="D42" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="7" t="n">
-        <v>0.845833333332848</v>
-      </c>
-      <c r="F42" s="7" t="n">
-        <v>0.860416666662786</v>
-      </c>
-      <c r="G42" s="6" t="n">
+      <c r="E42" s="7">
+        <v>0.84583333333284805</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0.86041666666278604</v>
+      </c>
+      <c r="G42" s="6">
         <v>3</v>
       </c>
-      <c r="H42" s="6" t="n">
+      <c r="H42" s="6">
         <v>3</v>
       </c>
-      <c r="I42" s="6" t="n">
+      <c r="I42" s="6">
         <v>3</v>
       </c>
       <c r="J42" s="6" t="s">
@@ -3042,11 +3244,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="9" t="n">
-        <v>45604.5226946296</v>
-      </c>
-      <c r="B43" s="10" t="n">
+    <row r="43" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>45604.522694629602</v>
+      </c>
+      <c r="B43" s="10">
         <v>45530</v>
       </c>
       <c r="C43" s="11" t="s">
@@ -3055,19 +3257,19 @@
       <c r="D43" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="12" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F43" s="12" t="n">
-        <v>0.427083333335759</v>
-      </c>
-      <c r="G43" s="11" t="n">
+      <c r="E43" s="12">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F43" s="12">
+        <v>0.42708333333575899</v>
+      </c>
+      <c r="G43" s="11">
         <v>35</v>
       </c>
-      <c r="H43" s="11" t="n">
+      <c r="H43" s="11">
         <v>9</v>
       </c>
-      <c r="I43" s="11" t="n">
+      <c r="I43" s="11">
         <v>7</v>
       </c>
       <c r="J43" s="11" t="s">
@@ -3092,11 +3294,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="n">
-        <v>45604.5270334607</v>
-      </c>
-      <c r="B44" s="5" t="n">
+    <row r="44" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>45604.527033460698</v>
+      </c>
+      <c r="B44" s="5">
         <v>45530</v>
       </c>
       <c r="C44" s="6" t="s">
@@ -3106,11 +3308,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9" t="n">
-        <v>45604.5278220255</v>
-      </c>
-      <c r="B45" s="10" t="n">
+    <row r="45" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="9">
+        <v>45604.527822025499</v>
+      </c>
+      <c r="B45" s="10">
         <v>45530</v>
       </c>
       <c r="C45" s="11" t="s">
@@ -3119,19 +3321,19 @@
       <c r="D45" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="12" t="n">
-        <v>0.840277777781012</v>
-      </c>
-      <c r="F45" s="12" t="n">
+      <c r="E45" s="12">
+        <v>0.84027777778101198</v>
+      </c>
+      <c r="F45" s="12">
         <v>0.84375</v>
       </c>
-      <c r="G45" s="11" t="n">
+      <c r="G45" s="11">
         <v>2</v>
       </c>
-      <c r="H45" s="11" t="n">
+      <c r="H45" s="11">
         <v>3</v>
       </c>
-      <c r="I45" s="11" t="n">
+      <c r="I45" s="11">
         <v>2</v>
       </c>
       <c r="J45" s="11" t="s">
@@ -3156,11 +3358,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="n">
-        <v>45604.5319776968</v>
-      </c>
-      <c r="B46" s="5" t="n">
+    <row r="46" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>45604.531977696803</v>
+      </c>
+      <c r="B46" s="5">
         <v>45531</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -3169,19 +3371,19 @@
       <c r="D46" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F46" s="7" t="n">
+      <c r="E46" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F46" s="7">
         <v>0.413888888884685</v>
       </c>
-      <c r="G46" s="6" t="n">
+      <c r="G46" s="6">
         <v>37</v>
       </c>
-      <c r="H46" s="6" t="n">
+      <c r="H46" s="6">
         <v>9</v>
       </c>
-      <c r="I46" s="6" t="n">
+      <c r="I46" s="6">
         <v>7</v>
       </c>
       <c r="J46" s="6" t="s">
@@ -3206,11 +3408,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="9" t="n">
-        <v>45604.5328435648</v>
-      </c>
-      <c r="B47" s="10" t="n">
+    <row r="47" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A47" s="9">
+        <v>45604.532843564797</v>
+      </c>
+      <c r="B47" s="10">
         <v>45531</v>
       </c>
       <c r="C47" s="11" t="s">
@@ -3219,19 +3421,19 @@
       <c r="D47" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E47" s="12" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="F47" s="12" t="n">
-        <v>0.720833333332848</v>
-      </c>
-      <c r="G47" s="11" t="n">
+      <c r="E47" s="12">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="F47" s="12">
+        <v>0.72083333333284805</v>
+      </c>
+      <c r="G47" s="11">
         <v>4</v>
       </c>
-      <c r="H47" s="11" t="n">
+      <c r="H47" s="11">
         <v>9</v>
       </c>
-      <c r="I47" s="11" t="n">
+      <c r="I47" s="11">
         <v>4</v>
       </c>
       <c r="J47" s="11" t="s">
@@ -3256,11 +3458,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="n">
-        <v>45604.533628125</v>
-      </c>
-      <c r="B48" s="5" t="n">
+    <row r="48" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>45604.533628124998</v>
+      </c>
+      <c r="B48" s="5">
         <v>45531</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -3269,19 +3471,19 @@
       <c r="D48" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E48" s="7" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="F48" s="7" t="n">
-        <v>0.864583333335759</v>
-      </c>
-      <c r="G48" s="6" t="n">
+      <c r="E48" s="7">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0.86458333333575899</v>
+      </c>
+      <c r="G48" s="6">
         <v>4</v>
       </c>
-      <c r="H48" s="6" t="n">
+      <c r="H48" s="6">
         <v>3</v>
       </c>
-      <c r="I48" s="6" t="n">
+      <c r="I48" s="6">
         <v>3</v>
       </c>
       <c r="J48" s="6" t="s">
@@ -3306,11 +3508,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="9" t="n">
-        <v>45597.1430211574</v>
-      </c>
-      <c r="B49" s="10" t="n">
+    <row r="49" spans="1:23" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="9">
+        <v>45597.143021157397</v>
+      </c>
+      <c r="B49" s="10">
         <v>45532</v>
       </c>
       <c r="C49" s="11" t="s">
@@ -3319,19 +3521,19 @@
       <c r="D49" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="12" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F49" s="12" t="n">
+      <c r="E49" s="12">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F49" s="12">
         <v>0.4375</v>
       </c>
-      <c r="G49" s="11" t="n">
+      <c r="G49" s="11">
         <v>45</v>
       </c>
-      <c r="H49" s="11" t="n">
+      <c r="H49" s="11">
         <v>10</v>
       </c>
-      <c r="I49" s="11" t="n">
+      <c r="I49" s="11">
         <v>8</v>
       </c>
       <c r="J49" s="11" t="s">
@@ -3359,11 +3561,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="n">
-        <v>45597.1442147685</v>
-      </c>
-      <c r="B50" s="5" t="n">
+    <row r="50" spans="1:23" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>45597.144214768501</v>
+      </c>
+      <c r="B50" s="5">
         <v>45532</v>
       </c>
       <c r="C50" s="6" t="s">
@@ -3372,19 +3574,19 @@
       <c r="D50" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="7" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="F50" s="7" t="n">
+      <c r="E50" s="7">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="F50" s="7">
         <v>0.71875</v>
       </c>
-      <c r="G50" s="6" t="n">
+      <c r="G50" s="6">
         <v>3</v>
       </c>
-      <c r="H50" s="6" t="n">
+      <c r="H50" s="6">
         <v>10</v>
       </c>
-      <c r="I50" s="6" t="n">
+      <c r="I50" s="6">
         <v>2</v>
       </c>
       <c r="J50" s="6" t="s">
@@ -3412,11 +3614,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9" t="n">
-        <v>45597.1447688773</v>
-      </c>
-      <c r="B51" s="10" t="n">
+    <row r="51" spans="1:23" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A51" s="9">
+        <v>45597.144768877297</v>
+      </c>
+      <c r="B51" s="10">
         <v>45532</v>
       </c>
       <c r="C51" s="11" t="s">
@@ -3425,19 +3627,19 @@
       <c r="D51" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E51" s="12" t="n">
-        <v>0.833333333335759</v>
-      </c>
-      <c r="F51" s="12" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="G51" s="11" t="n">
+      <c r="E51" s="12">
+        <v>0.83333333333575899</v>
+      </c>
+      <c r="F51" s="12">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="G51" s="11">
         <v>7</v>
       </c>
-      <c r="H51" s="11" t="n">
+      <c r="H51" s="11">
         <v>3</v>
       </c>
-      <c r="I51" s="11" t="n">
+      <c r="I51" s="11">
         <v>3</v>
       </c>
       <c r="J51" s="11" t="s">
@@ -3462,11 +3664,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="n">
-        <v>45551.7802770949</v>
-      </c>
-      <c r="B52" s="5" t="n">
+    <row r="52" spans="1:23" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>45551.780277094898</v>
+      </c>
+      <c r="B52" s="5">
         <v>45533</v>
       </c>
       <c r="C52" s="6" t="s">
@@ -3475,13 +3677,13 @@
       <c r="D52" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E52" s="7" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="F52" s="7" t="n">
-        <v>0.416666666664241</v>
-      </c>
-      <c r="G52" s="6" t="n">
+      <c r="E52" s="7">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="F52" s="7">
+        <v>0.41666666666424101</v>
+      </c>
+      <c r="G52" s="6">
         <v>36</v>
       </c>
       <c r="H52" s="6" t="s">
@@ -3515,11 +3717,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="15" t="n">
+    <row r="53" spans="1:23" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A53" s="15">
         <v>45597.1455984606</v>
       </c>
-      <c r="B53" s="16" t="n">
+      <c r="B53" s="16">
         <v>45533</v>
       </c>
       <c r="C53" s="17" t="s">
@@ -3528,19 +3730,19 @@
       <c r="D53" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="18" t="n">
+      <c r="E53" s="18">
         <v>0.84375</v>
       </c>
-      <c r="F53" s="18" t="n">
-        <v>0.864583333335759</v>
-      </c>
-      <c r="G53" s="17" t="n">
+      <c r="F53" s="18">
+        <v>0.86458333333575899</v>
+      </c>
+      <c r="G53" s="17">
         <v>5</v>
       </c>
-      <c r="H53" s="17" t="n">
+      <c r="H53" s="17">
         <v>3</v>
       </c>
-      <c r="I53" s="17" t="n">
+      <c r="I53" s="17">
         <v>3</v>
       </c>
       <c r="J53" s="17" t="s">
@@ -3565,7 +3767,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="20"/>
       <c r="B54" s="21"/>
       <c r="C54" s="22"/>
@@ -3590,7 +3792,7 @@
       <c r="V54" s="27"/>
       <c r="W54" s="27"/>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="28"/>
       <c r="B55" s="29"/>
       <c r="C55" s="30"/>
@@ -3615,7 +3817,7 @@
       <c r="V55" s="27"/>
       <c r="W55" s="27"/>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="20"/>
       <c r="B56" s="21"/>
       <c r="C56" s="22"/>
@@ -3640,7 +3842,7 @@
       <c r="V56" s="27"/>
       <c r="W56" s="27"/>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="28"/>
       <c r="B57" s="29"/>
       <c r="C57" s="30"/>
@@ -3665,7 +3867,7 @@
       <c r="V57" s="27"/>
       <c r="W57" s="27"/>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="20"/>
       <c r="B58" s="21"/>
       <c r="C58" s="22"/>
@@ -3690,7 +3892,7 @@
       <c r="V58" s="27"/>
       <c r="W58" s="27"/>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
       <c r="B59" s="29"/>
       <c r="C59" s="30"/>
@@ -3715,7 +3917,7 @@
       <c r="V59" s="27"/>
       <c r="W59" s="27"/>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="20"/>
       <c r="B60" s="21"/>
       <c r="C60" s="22"/>
@@ -3740,7 +3942,7 @@
       <c r="V60" s="27"/>
       <c r="W60" s="27"/>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
       <c r="B61" s="29"/>
       <c r="C61" s="30"/>
@@ -3765,7 +3967,7 @@
       <c r="V61" s="27"/>
       <c r="W61" s="27"/>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="20"/>
       <c r="B62" s="21"/>
       <c r="C62" s="22"/>
@@ -3790,7 +3992,7 @@
       <c r="V62" s="27"/>
       <c r="W62" s="27"/>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
       <c r="B63" s="29"/>
       <c r="C63" s="30"/>
@@ -3815,7 +4017,7 @@
       <c r="V63" s="27"/>
       <c r="W63" s="27"/>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="20"/>
       <c r="B64" s="21"/>
       <c r="C64" s="22"/>
@@ -3840,7 +4042,7 @@
       <c r="V64" s="27"/>
       <c r="W64" s="27"/>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="28"/>
       <c r="B65" s="29"/>
       <c r="C65" s="30"/>
@@ -3865,7 +4067,7 @@
       <c r="V65" s="27"/>
       <c r="W65" s="27"/>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="20"/>
       <c r="B66" s="21"/>
       <c r="C66" s="22"/>
@@ -3891,14 +4093,9 @@
       <c r="W66" s="27"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <tableParts>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -3907,656 +4104,646 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B12:R24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="38" t="n">
-        <v>45518.6936316782</v>
-      </c>
-      <c r="C12" s="39" t="n">
+    <row r="12" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B12" s="38">
+        <v>45518.693631678201</v>
+      </c>
+      <c r="C12" s="39">
         <v>45512</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="41" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="G12" s="41" t="n">
+      <c r="F12" s="40">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="G12" s="40">
         <v>0.375</v>
       </c>
-      <c r="H12" s="40" t="n">
+      <c r="H12" s="27">
         <v>34</v>
       </c>
-      <c r="I12" s="40" t="n">
+      <c r="I12" s="27">
         <v>10</v>
       </c>
-      <c r="J12" s="40" t="n">
+      <c r="J12" s="27">
         <v>10</v>
       </c>
-      <c r="K12" s="40" t="s">
+      <c r="K12" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="40" t="s">
+      <c r="L12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O12" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="P12" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q12" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="R12" s="40" t="s">
+      <c r="N12" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" s="27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="38" t="n">
-        <v>45551.7786426273</v>
-      </c>
-      <c r="C13" s="39" t="n">
+    <row r="13" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B13" s="38">
+        <v>45551.778642627301</v>
+      </c>
+      <c r="C13" s="39">
         <v>45512</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="41" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="G13" s="41" t="n">
+      <c r="F13" s="40">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="G13" s="40">
         <v>0.711805555554747</v>
       </c>
-      <c r="H13" s="40" t="n">
+      <c r="H13" s="27">
         <v>4</v>
       </c>
-      <c r="I13" s="40" t="n">
+      <c r="I13" s="27">
         <v>10</v>
       </c>
-      <c r="J13" s="40" t="n">
+      <c r="J13" s="27">
         <v>1</v>
       </c>
-      <c r="K13" s="40" t="s">
+      <c r="K13" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="40" t="s">
+      <c r="L13" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="40" t="s">
+      <c r="M13" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="N13" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" s="40" t="s">
+      <c r="N13" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="P13" s="40" t="s">
+      <c r="P13" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="Q13" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="R13" s="40" t="s">
+      <c r="Q13" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="38" t="n">
-        <v>45585.536269294</v>
-      </c>
-      <c r="C14" s="39" t="n">
+    <row r="14" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B14" s="38">
+        <v>45585.536269294003</v>
+      </c>
+      <c r="C14" s="39">
         <v>45512</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="41" t="n">
-        <v>0.840277777781012</v>
-      </c>
-      <c r="G14" s="41" t="n">
+      <c r="F14" s="40">
+        <v>0.84027777778101198</v>
+      </c>
+      <c r="G14" s="40">
         <v>0.850694444445253</v>
       </c>
-      <c r="H14" s="40" t="n">
+      <c r="H14" s="27">
         <v>5</v>
       </c>
-      <c r="I14" s="40" t="n">
+      <c r="I14" s="27">
         <v>3</v>
       </c>
-      <c r="J14" s="40" t="n">
+      <c r="J14" s="27">
         <v>2</v>
       </c>
-      <c r="K14" s="40" t="s">
+      <c r="K14" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="40" t="s">
+      <c r="L14" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="M14" s="40" t="s">
+      <c r="M14" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="N14" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="O14" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="P14" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q14" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="R14" s="40" t="s">
+      <c r="N14" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="O14" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="R14" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="38" t="n">
-        <v>45551.7802770949</v>
-      </c>
-      <c r="C15" s="39" t="n">
+    <row r="15" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B15" s="38">
+        <v>45551.780277094898</v>
+      </c>
+      <c r="C15" s="39">
         <v>45513</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="41" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="G15" s="41" t="n">
-        <v>0.416666666664241</v>
-      </c>
-      <c r="H15" s="40" t="n">
+      <c r="F15" s="40">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="G15" s="40">
+        <v>0.41666666666424101</v>
+      </c>
+      <c r="H15" s="27">
         <v>36</v>
       </c>
-      <c r="I15" s="40" t="s">
+      <c r="I15" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="40" t="s">
+      <c r="J15" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="K15" s="40" t="s">
+      <c r="K15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="40" t="s">
+      <c r="L15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="M15" s="40" t="s">
+      <c r="M15" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="N15" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="O15" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="P15" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q15" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="R15" s="40" t="s">
+      <c r="N15" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="P15" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="38" t="n">
-        <v>45551.7814166204</v>
-      </c>
-      <c r="C16" s="39" t="n">
+    <row r="16" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B16" s="38">
+        <v>45551.781416620397</v>
+      </c>
+      <c r="C16" s="39">
         <v>45513</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="41" t="n">
+      <c r="F16" s="40">
         <v>0.84375</v>
       </c>
-      <c r="G16" s="41" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="H16" s="40" t="n">
+      <c r="G16" s="40">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="H16" s="27">
         <v>4</v>
       </c>
-      <c r="I16" s="40" t="n">
+      <c r="I16" s="27">
         <v>3</v>
       </c>
-      <c r="J16" s="40" t="n">
+      <c r="J16" s="27">
         <v>2</v>
       </c>
-      <c r="K16" s="40" t="s">
+      <c r="K16" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="40" t="s">
+      <c r="L16" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="M16" s="40" t="s">
+      <c r="M16" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="N16" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O16" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="P16" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q16" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="R16" s="40" t="s">
+      <c r="N16" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="P16" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="38" t="n">
-        <v>45585.5372411921</v>
-      </c>
-      <c r="C17" s="39" t="n">
+    <row r="17" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B17" s="38">
+        <v>45585.537241192098</v>
+      </c>
+      <c r="C17" s="39">
         <v>45513</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="41" t="n">
-        <v>0.708333333335759</v>
-      </c>
-      <c r="G17" s="41" t="n">
-        <v>0.718055555553292</v>
-      </c>
-      <c r="H17" s="40" t="n">
+      <c r="F17" s="40">
+        <v>0.70833333333575899</v>
+      </c>
+      <c r="G17" s="40">
+        <v>0.71805555555329204</v>
+      </c>
+      <c r="H17" s="27">
         <v>2</v>
       </c>
-      <c r="I17" s="40" t="n">
+      <c r="I17" s="27">
         <v>10</v>
       </c>
-      <c r="J17" s="40" t="n">
+      <c r="J17" s="27">
         <v>2</v>
       </c>
-      <c r="K17" s="40" t="s">
+      <c r="K17" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="40" t="s">
+      <c r="L17" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="M17" s="40" t="s">
+      <c r="M17" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O17" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="P17" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q17" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="R17" s="40" t="s">
+      <c r="N17" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="P17" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="38" t="n">
-        <v>45585.5382381134</v>
-      </c>
-      <c r="C18" s="39" t="n">
+    <row r="18" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B18" s="38">
+        <v>45585.538238113397</v>
+      </c>
+      <c r="C18" s="39">
         <v>45514</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="41" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="G18" s="41" t="n">
-        <v>0.361111111109494</v>
-      </c>
-      <c r="H18" s="40" t="n">
+      <c r="F18" s="40">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="G18" s="40">
+        <v>0.36111111110949401</v>
+      </c>
+      <c r="H18" s="27">
         <v>7</v>
       </c>
-      <c r="I18" s="40" t="n">
+      <c r="I18" s="27">
         <v>6</v>
       </c>
-      <c r="J18" s="40" t="n">
+      <c r="J18" s="27">
         <v>6</v>
       </c>
-      <c r="K18" s="40" t="s">
+      <c r="K18" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="40" t="s">
+      <c r="L18" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="N18" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="O18" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="P18" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q18" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="R18" s="40" t="s">
+      <c r="N18" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="P18" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q18" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="R18" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="38" t="n">
-        <v>45585.5398058333</v>
-      </c>
-      <c r="C19" s="39" t="n">
+    <row r="19" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B19" s="38">
+        <v>45585.539805833301</v>
+      </c>
+      <c r="C19" s="39">
         <v>45514</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="41" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="G19" s="41" t="n">
-        <v>0.864583333335759</v>
-      </c>
-      <c r="H19" s="40" t="n">
+      <c r="F19" s="40">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="G19" s="40">
+        <v>0.86458333333575899</v>
+      </c>
+      <c r="H19" s="27">
         <v>4</v>
       </c>
-      <c r="I19" s="40" t="n">
+      <c r="I19" s="27">
         <v>3</v>
       </c>
-      <c r="J19" s="40" t="n">
+      <c r="J19" s="27">
         <v>3</v>
       </c>
-      <c r="K19" s="40" t="s">
+      <c r="K19" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="40" t="s">
+      <c r="L19" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N19" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O19" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="P19" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q19" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="R19" s="40" t="s">
+      <c r="N19" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="R19" s="27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="38" t="n">
-        <v>45585.5508097222</v>
-      </c>
-      <c r="C20" s="39" t="n">
+    <row r="20" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B20" s="38">
+        <v>45585.550809722197</v>
+      </c>
+      <c r="C20" s="39">
         <v>45515</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="41" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="G20" s="41" t="n">
+      <c r="F20" s="40">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="G20" s="40">
         <v>0.350694444445253</v>
       </c>
-      <c r="H20" s="40" t="n">
+      <c r="H20" s="27">
         <v>7</v>
       </c>
-      <c r="I20" s="40" t="n">
+      <c r="I20" s="27">
         <v>6</v>
       </c>
-      <c r="J20" s="40" t="n">
+      <c r="J20" s="27">
         <v>6</v>
       </c>
-      <c r="K20" s="40" t="s">
+      <c r="K20" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="40" t="s">
+      <c r="L20" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="N20" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="O20" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="P20" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q20" s="40" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="38" t="n">
-        <v>45585.5517788889</v>
-      </c>
-      <c r="C21" s="39" t="n">
+      <c r="N20" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q20" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B21" s="38">
+        <v>45585.551778888897</v>
+      </c>
+      <c r="C21" s="39">
         <v>45515</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="41" t="n">
+      <c r="F21" s="40">
         <v>0.84375</v>
       </c>
-      <c r="G21" s="41" t="n">
-        <v>0.854166666664241</v>
-      </c>
-      <c r="H21" s="40" t="n">
+      <c r="G21" s="40">
+        <v>0.85416666666424101</v>
+      </c>
+      <c r="H21" s="27">
         <v>3</v>
       </c>
-      <c r="I21" s="40" t="n">
+      <c r="I21" s="27">
         <v>3</v>
       </c>
-      <c r="J21" s="40" t="n">
+      <c r="J21" s="27">
         <v>2</v>
       </c>
-      <c r="K21" s="40" t="s">
+      <c r="K21" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="L21" s="40" t="s">
+      <c r="L21" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="M21" s="40" t="s">
+      <c r="M21" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="N21" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O21" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="P21" s="40" t="s">
+      <c r="N21" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="Q21" s="40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="38" t="n">
+      <c r="Q21" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B22" s="38">
         <v>45585.5539274537</v>
       </c>
-      <c r="C22" s="39" t="n">
+      <c r="C22" s="39">
         <v>45516</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="41" t="n">
-        <v>0.333333333335759</v>
-      </c>
-      <c r="G22" s="41" t="n">
-        <v>0.427083333335759</v>
-      </c>
-      <c r="H22" s="40" t="n">
+      <c r="F22" s="40">
+        <v>0.33333333333575899</v>
+      </c>
+      <c r="G22" s="40">
+        <v>0.42708333333575899</v>
+      </c>
+      <c r="H22" s="27">
         <v>35</v>
       </c>
-      <c r="I22" s="40" t="n">
+      <c r="I22" s="27">
         <v>9</v>
       </c>
-      <c r="J22" s="40" t="n">
+      <c r="J22" s="27">
         <v>7</v>
       </c>
-      <c r="K22" s="40" t="s">
+      <c r="K22" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="L22" s="40" t="s">
+      <c r="L22" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="M22" s="40" t="s">
+      <c r="M22" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="N22" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="O22" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="P22" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q22" s="40" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="38" t="n">
-        <v>45585.5553327199</v>
-      </c>
-      <c r="C23" s="39" t="n">
+      <c r="N22" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="P22" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q22" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B23" s="38">
+        <v>45585.555332719901</v>
+      </c>
+      <c r="C23" s="39">
         <v>45516</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="R23" s="40" t="s">
+      <c r="R23" s="27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="38" t="n">
-        <v>45585.5619040509</v>
-      </c>
-      <c r="C24" s="39" t="n">
+    <row r="24" spans="2:18" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B24" s="38">
+        <v>45585.561904050897</v>
+      </c>
+      <c r="C24" s="39">
         <v>45516</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="41" t="n">
-        <v>0.840277777781012</v>
-      </c>
-      <c r="G24" s="41" t="n">
+      <c r="F24" s="40">
+        <v>0.84027777778101198</v>
+      </c>
+      <c r="G24" s="40">
         <v>0.84375</v>
       </c>
-      <c r="H24" s="40" t="n">
+      <c r="H24" s="27">
         <v>2</v>
       </c>
-      <c r="I24" s="40" t="n">
+      <c r="I24" s="27">
         <v>3</v>
       </c>
-      <c r="J24" s="40" t="n">
+      <c r="J24" s="27">
         <v>3</v>
       </c>
-      <c r="K24" s="40" t="s">
+      <c r="K24" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="L24" s="40" t="s">
+      <c r="L24" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="N24" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O24" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="P24" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q24" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="R24" s="40" t="s">
+      <c r="N24" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="P24" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="R24" s="27" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <tableParts>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>

</xml_diff>